<commit_message>
Agregado diagrama de base de datos y funcion para formatear el var_dump
</commit_message>
<xml_diff>
--- a/EquiposYVuelos.xlsx
+++ b/EquiposYVuelos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arust\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agonz\Source\Repos\Progra Web 2\tp\public_html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5E6243-3942-408C-8D97-744502D9CE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA84D608-0447-47AA-B3E6-F88A0C615ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Equipos" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="135">
   <si>
     <t>Modelo</t>
   </si>
@@ -328,9 +328,6 @@
     <t>Entre Destinos</t>
   </si>
   <si>
-    <t>Circuito 1</t>
-  </si>
-  <si>
     <t>EEI</t>
   </si>
   <si>
@@ -343,9 +340,6 @@
     <t>Marte</t>
   </si>
   <si>
-    <t>Circuito 2</t>
-  </si>
-  <si>
     <t>Ganimedes</t>
   </si>
   <si>
@@ -425,6 +419,18 @@
   </si>
   <si>
     <t>G50,S50</t>
+  </si>
+  <si>
+    <t>Modelos</t>
+  </si>
+  <si>
+    <t>nave_espacial</t>
+  </si>
+  <si>
+    <t>Buenos aires</t>
+  </si>
+  <si>
+    <t>Ankara</t>
   </si>
 </sst>
 </file>
@@ -462,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -498,11 +504,57 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -510,8 +562,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -792,18 +855,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="D1" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -829,7 +906,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -855,7 +932,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -881,7 +958,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -901,13 +978,13 @@
         <v>21</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="I5" s="2">
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -933,7 +1010,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -959,7 +1036,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
@@ -985,7 +1062,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1011,7 +1088,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1114,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1063,7 +1140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1174,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -1108,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
@@ -1116,7 +1193,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1124,7 +1201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1217,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1148,7 +1225,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1156,7 +1233,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -1164,7 +1241,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>9</v>
       </c>
@@ -1172,7 +1249,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1180,7 +1257,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1188,7 +1265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1196,7 +1273,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1204,7 +1281,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1212,7 +1289,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1297,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1228,7 +1305,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1236,7 +1313,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1244,7 +1321,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>13</v>
       </c>
@@ -1252,7 +1329,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>13</v>
       </c>
@@ -1260,7 +1337,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>13</v>
       </c>
@@ -1268,7 +1345,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>13</v>
       </c>
@@ -1276,7 +1353,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>15</v>
       </c>
@@ -1284,7 +1361,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
@@ -1292,7 +1369,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -1300,7 +1377,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>15</v>
       </c>
@@ -1308,7 +1385,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>14</v>
       </c>
@@ -1316,7 +1393,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -1324,7 +1401,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>14</v>
       </c>
@@ -1332,7 +1409,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>14</v>
       </c>
@@ -1340,7 +1417,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>14</v>
       </c>
@@ -1348,7 +1425,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1356,7 +1433,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -1364,7 +1441,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
@@ -1376,6 +1453,10 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:B48">
     <sortCondition ref="A3:A48"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1383,354 +1464,357 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:I27"/>
+  <dimension ref="C3:K28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="4" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="1">
+      <c r="D5" s="1">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="1">
+      <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B6" s="1">
+      <c r="D7" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="1">
+      <c r="D8" s="1">
         <v>5</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B8" s="1">
+      <c r="D9" s="1">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="1">
+      <c r="D10" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="1">
+      <c r="D11" s="1">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="F20" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="6" t="s">
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="6" t="s">
+      <c r="G23" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="H23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="E24" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F21" s="1" t="s">
+      <c r="F25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G24" s="1" t="s">
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>128</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="I24" s="1" t="s">
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="C19:G19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>